<commit_message>
choice test list update csv - add 12 more choices (18 total)
</commit_message>
<xml_diff>
--- a/lists/rewardconfidencelist_study4_base.xlsx
+++ b/lists/rewardconfidencelist_study4_base.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gelliott/Documents/projects/delaylearn/feedback-delay-four/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65BC2F9A-E7CA-2848-95AB-F48E851AB2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557C2184-E238-DF4B-A229-74FAB531A52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="5400" windowWidth="31880" windowHeight="19340"/>
+    <workbookView xWindow="2680" yWindow="760" windowWidth="31880" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rewardconfidencelist_study4_bas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>trial</t>
   </si>
@@ -54,11 +66,17 @@
   <si>
     <t>random</t>
   </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -195,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +391,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -536,8 +560,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -892,54 +917,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="8" width="25" customWidth="1"/>
+    <col min="9" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
@@ -950,36 +981,42 @@
         <v>1</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <f>IF(I2=0,C2,D2)</f>
+      <c r="G2">
+        <f t="shared" ref="G2:G19" si="0">IF(K2=0,E2,F2)</f>
         <v>2</v>
       </c>
-      <c r="F2">
-        <f>IF(I2=0,D2,C2)</f>
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(I2=0,CONCATENATE("images/choice_trial_",C2,".png"),CONCATENATE("images/choice_trial_",D2,".png"))</f>
+      <c r="H2">
+        <f t="shared" ref="H2:H19" si="1">IF(K2=0,F2,E2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I19" si="2">IF(K2=0,CONCATENATE("images/choice_trial_",E2,".png"),CONCATENATE("images/choice_trial_",F2,".png"))</f>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="H2" t="str">
-        <f>IF(I2=0,CONCATENATE("images/choice_trial_",D2,".png"),CONCATENATE("images/choice_trial_",C2,".png"))</f>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J19" si="3">IF(K2=0,CONCATENATE("images/choice_trial_",F2,".png"),CONCATENATE("images/choice_trial_",E2,".png"))</f>
         <v>images/choice_trial_1.png</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <f ca="1">RAND()</f>
-        <v>0.50416683710921639</v>
+        <v>0.98150669107872668</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -987,39 +1024,45 @@
         <v>2</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>6</v>
       </c>
-      <c r="E3">
-        <f>IF(I3=0,C3,D3)</f>
+      <c r="G3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F3">
-        <f>IF(I3=0,D3,C3)</f>
+      <c r="H3">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G3" t="str">
-        <f>IF(I3=0,CONCATENATE("images/choice_trial_",C3,".png"),CONCATENATE("images/choice_trial_",D3,".png"))</f>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_5.png</v>
       </c>
-      <c r="H3" t="str">
-        <f>IF(I3=0,CONCATENATE("images/choice_trial_",D3,".png"),CONCATENATE("images/choice_trial_",C3,".png"))</f>
+      <c r="J3" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_6.png</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K13" ca="1" si="0">RAND()</f>
-        <v>0.88177594374928614</v>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M19" ca="1" si="4">RAND()</f>
+        <v>0.41259763757567858</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1027,39 +1070,45 @@
         <v>3</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>8</v>
       </c>
-      <c r="E4">
-        <f>IF(I4=0,C4,D4)</f>
+      <c r="G4">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F4">
-        <f>IF(I4=0,D4,C4)</f>
+      <c r="H4">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G4" t="str">
-        <f>IF(I4=0,CONCATENATE("images/choice_trial_",C4,".png"),CONCATENATE("images/choice_trial_",D4,".png"))</f>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="H4" t="str">
-        <f>IF(I4=0,CONCATENATE("images/choice_trial_",D4,".png"),CONCATENATE("images/choice_trial_",C4,".png"))</f>
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_7.png</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
       <c r="K4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.17132577667354509</v>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.10438337151439081</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1067,39 +1116,45 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>10</v>
       </c>
-      <c r="E5">
-        <f>IF(I5=0,C5,D5)</f>
+      <c r="G5">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F5">
-        <f>IF(I5=0,D5,C5)</f>
+      <c r="H5">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G5" t="str">
-        <f>IF(I5=0,CONCATENATE("images/choice_trial_",C5,".png"),CONCATENATE("images/choice_trial_",D5,".png"))</f>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="H5" t="str">
-        <f>IF(I5=0,CONCATENATE("images/choice_trial_",D5,".png"),CONCATENATE("images/choice_trial_",C5,".png"))</f>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58291695772190111</v>
+      <c r="M5">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.95502430321302889</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1107,39 +1162,45 @@
         <v>5</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>12</v>
       </c>
-      <c r="E6">
-        <f>IF(I6=0,C6,D6)</f>
+      <c r="G6">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F6">
-        <f>IF(I6=0,D6,C6)</f>
+      <c r="H6">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G6" t="str">
-        <f>IF(I6=0,CONCATENATE("images/choice_trial_",C6,".png"),CONCATENATE("images/choice_trial_",D6,".png"))</f>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="H6" t="str">
-        <f>IF(I6=0,CONCATENATE("images/choice_trial_",D6,".png"),CONCATENATE("images/choice_trial_",C6,".png"))</f>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_11.png</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="K6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.75446728820366749</v>
+      <c r="M6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.4314064148488157</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1147,263 +1208,623 @@
         <v>6</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>14</v>
       </c>
-      <c r="E7">
-        <f>IF(I7=0,C7,D7)</f>
+      <c r="G7">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F7">
-        <f>IF(I7=0,D7,C7)</f>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G7" t="str">
-        <f>IF(I7=0,CONCATENATE("images/choice_trial_",C7,".png"),CONCATENATE("images/choice_trial_",D7,".png"))</f>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_13.png</v>
       </c>
-      <c r="H7" t="str">
-        <f>IF(I7=0,CONCATENATE("images/choice_trial_",D7,".png"),CONCATENATE("images/choice_trial_",C7,".png"))</f>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_14.png</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.48250577261269856</v>
+      <c r="M7">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.45962968354286493</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="E8" s="1">
+        <f>E2</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f>F3</f>
         <v>6</v>
       </c>
-      <c r="E8">
-        <f>IF(I8=0,C8,D8)</f>
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f>IF(I8=0,D8,C8)</f>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G8" t="str">
-        <f>IF(I8=0,CONCATENATE("images/choice_trial_",C8,".png"),CONCATENATE("images/choice_trial_",D8,".png"))</f>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_1.png</v>
       </c>
-      <c r="H8" t="str">
-        <f>IF(I8=0,CONCATENATE("images/choice_trial_",D8,".png"),CONCATENATE("images/choice_trial_",C8,".png"))</f>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_6.png</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <f ca="1">RAND()</f>
-        <v>0.63114126667135417</v>
+        <v>0.88443957669906159</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
       <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>23</v>
       </c>
-      <c r="C9">
+      <c r="E9" s="1">
+        <f>E3</f>
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="F9" s="1">
+        <f>F4</f>
         <v>8</v>
       </c>
-      <c r="E9">
-        <f>IF(I9=0,C9,D9)</f>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F9">
-        <f>IF(I9=0,D9,C9)</f>
+      <c r="H9">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G9" t="str">
-        <f>IF(I9=0,CONCATENATE("images/choice_trial_",C9,".png"),CONCATENATE("images/choice_trial_",D9,".png"))</f>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="H9" t="str">
-        <f>IF(I9=0,CONCATENATE("images/choice_trial_",D9,".png"),CONCATENATE("images/choice_trial_",C9,".png"))</f>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_5.png</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
       <c r="K9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7294895647535341</v>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.58426786251519292</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>11</v>
+      </c>
       <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="E10" s="1">
+        <f>E4</f>
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="F10" s="1">
+        <f>F2</f>
         <v>2</v>
       </c>
-      <c r="E10">
-        <f>IF(I10=0,C10,D10)</f>
+      <c r="G10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F10">
-        <f>IF(I10=0,D10,C10)</f>
+      <c r="H10">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G10" t="str">
-        <f>IF(I10=0,CONCATENATE("images/choice_trial_",C10,".png"),CONCATENATE("images/choice_trial_",D10,".png"))</f>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_7.png</v>
       </c>
-      <c r="H10" t="str">
-        <f>IF(I10=0,CONCATENATE("images/choice_trial_",D10,".png"),CONCATENATE("images/choice_trial_",C10,".png"))</f>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.96123239786970283</v>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.31351725204183645</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
       <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>45</v>
       </c>
-      <c r="C11">
+      <c r="E11" s="1">
+        <f>E5</f>
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="F11" s="1">
+        <f>F6</f>
         <v>12</v>
       </c>
-      <c r="E11">
-        <f>IF(I11=0,C11,D11)</f>
+      <c r="G11">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F11">
-        <f>IF(I11=0,D11,C11)</f>
+      <c r="H11">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G11" t="str">
-        <f>IF(I11=0,CONCATENATE("images/choice_trial_",C11,".png"),CONCATENATE("images/choice_trial_",D11,".png"))</f>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="H11" t="str">
-        <f>IF(I11=0,CONCATENATE("images/choice_trial_",D11,".png"),CONCATENATE("images/choice_trial_",C11,".png"))</f>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3719030681314415E-2</v>
+      <c r="M11">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.90840979977287706</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>56</v>
       </c>
-      <c r="C12">
+      <c r="E12" s="1">
+        <f>E6</f>
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="F12" s="1">
+        <f>F7</f>
         <v>14</v>
       </c>
-      <c r="E12">
-        <f>IF(I12=0,C12,D12)</f>
+      <c r="G12">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F12">
-        <f>IF(I12=0,D12,C12)</f>
+      <c r="H12">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G12" t="str">
-        <f>IF(I12=0,CONCATENATE("images/choice_trial_",C12,".png"),CONCATENATE("images/choice_trial_",D12,".png"))</f>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_11.png</v>
       </c>
-      <c r="H12" t="str">
-        <f>IF(I12=0,CONCATENATE("images/choice_trial_",D12,".png"),CONCATENATE("images/choice_trial_",C12,".png"))</f>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_14.png</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.63546421092146321</v>
+      <c r="M12">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.34981033871906264</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>64</v>
       </c>
-      <c r="C13">
+      <c r="E13" s="1">
+        <f>E7</f>
         <v>13</v>
       </c>
-      <c r="D13">
+      <c r="F13" s="1">
+        <f>F5</f>
         <v>10</v>
       </c>
-      <c r="E13">
-        <f>IF(I13=0,C13,D13)</f>
+      <c r="G13">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F13">
-        <f>IF(I13=0,D13,C13)</f>
+      <c r="H13">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G13" t="str">
-        <f>IF(I13=0,CONCATENATE("images/choice_trial_",C13,".png"),CONCATENATE("images/choice_trial_",D13,".png"))</f>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="H13" t="str">
-        <f>IF(I13=0,CONCATENATE("images/choice_trial_",D13,".png"),CONCATENATE("images/choice_trial_",C13,".png"))</f>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
         <v>images/choice_trial_13.png</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32323229274221432</v>
+      <c r="M13">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.7423282874033328E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <f>E2</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E5</f>
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_1.png</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_9.png</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0.5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.71239856630367149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1">
+        <f>E3</f>
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E6</f>
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_11.png</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_5.png</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.2774466903581041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1">
+        <f>E4</f>
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E7</f>
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_7.png</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_13.png</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0.5</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.36259102097447726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <f>F2</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>F6</f>
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_12.png</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_2.png</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0.5</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.23559313741812482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>26</v>
+      </c>
+      <c r="E18" s="1">
+        <f>F3</f>
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <f>F7</f>
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_6.png</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_14.png</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0.5</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.33523483264971166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1">
+        <f>F4</f>
+        <v>8</v>
+      </c>
+      <c r="F19" s="1">
+        <f>F5</f>
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>images/choice_trial_10.png</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>images/choice_trial_8.png</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0.5</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.5751416948754946</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K7">
-    <sortCondition ref="B2:B7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M7">
+    <sortCondition ref="D2:D7"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>